<commit_message>
updates before new cad files
</commit_message>
<xml_diff>
--- a/docs/hardware/Helmoro_BoM_fasteners.xlsx
+++ b/docs/hardware/Helmoro_BoM_fasteners.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AHE\Documents\Git_Data\HelMoRo\docs\hardware\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{605207F9-48DA-4EEE-A783-2232A97AF58A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2802D8F8-36F2-44B8-8EAC-15485DAFEBEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26070" yWindow="2730" windowWidth="16035" windowHeight="10920" xr2:uid="{D43A7108-50A9-4FCF-900B-676A8BDC7C7C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{D43A7108-50A9-4FCF-900B-676A8BDC7C7C}"/>
   </bookViews>
   <sheets>
     <sheet name="BoM" sheetId="1" r:id="rId1"/>
@@ -44,9 +44,6 @@
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="59">
   <si>
     <t>QTY</t>
-  </si>
-  <si>
-    <t>DOCUMENT-NR.</t>
   </si>
   <si>
     <t>DESCRIPTION</t>
@@ -109,9 +106,6 @@
     <t>Total [CHF]</t>
   </si>
   <si>
-    <t>Price per unit (CHF)</t>
-  </si>
-  <si>
     <t>PEM CLA-M3-1 ---N</t>
   </si>
   <si>
@@ -140,9 +134,6 @@
   </si>
   <si>
     <t>Screws M3x18</t>
-  </si>
-  <si>
-    <t>HEL-06-01009-00</t>
   </si>
   <si>
     <t>Gewindebuchsen für Kunststoffe 003-M3</t>
@@ -184,9 +175,6 @@
     <t>Screw M2.5x16</t>
   </si>
   <si>
-    <t>HEL-05-03001-00</t>
-  </si>
-  <si>
     <t>Screw M3x4</t>
   </si>
   <si>
@@ -218,6 +206,18 @@
   </si>
   <si>
     <t>[Bossard](https://www.bossard.com/eshop/ch-en/screws/screws-and-bolts-with-internal-drive/hex-socket-head-cap-screws-fully-threaded/p/3/)</t>
+  </si>
+  <si>
+    <t>ISO 4762 M3x4</t>
+  </si>
+  <si>
+    <t>Thread Insert MULTISERT 003M3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PART NR. </t>
+  </si>
+  <si>
+    <t>PRICE PER UNIT (CHF)</t>
   </si>
 </sst>
 </file>
@@ -311,6 +311,25 @@
   </cellStyles>
   <dxfs count="585">
     <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Arial"/>
+        <family val="2"/>
+        <scheme val="none"/>
+      </font>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="0" formatCode="General"/>
     </dxf>
     <dxf>
@@ -567,25 +586,6 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Arial"/>
-        <family val="2"/>
-        <scheme val="none"/>
-      </font>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor rgb="FFFF0000"/>
@@ -4717,15 +4717,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC433D18-8D56-470A-8DB2-FE2100CD4686}" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15" totalsRowDxfId="14">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{AC433D18-8D56-470A-8DB2-FE2100CD4686}" name="Table1" displayName="Table1" ref="A1:F54" totalsRowShown="0" headerRowDxfId="0" dataDxfId="16" totalsRowDxfId="15">
   <autoFilter ref="A1:F54" xr:uid="{AB8CB7B2-62CE-4583-9267-907B832DB447}"/>
   <tableColumns count="6">
-    <tableColumn id="2" xr3:uid="{E4EF20A8-BAA7-4285-8E2C-1FF15F4D9DE0}" name="QTY" dataDxfId="13" totalsRowDxfId="12"/>
-    <tableColumn id="3" xr3:uid="{7C114C88-4C53-4A01-875E-42C9A5D3836B}" name="DOCUMENT-NR." dataDxfId="11" totalsRowDxfId="10"/>
-    <tableColumn id="4" xr3:uid="{F56A10FA-89C2-4781-AECC-93B30002C92E}" name="DESCRIPTION" dataDxfId="9" totalsRowDxfId="8"/>
-    <tableColumn id="6" xr3:uid="{15467916-B419-479D-A3A9-C6B2B5C762DF}" name="PRODUCT CODE" dataDxfId="7" totalsRowDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{2349CBB5-C81B-4DFD-9B9F-CC6E1EB0C9BF}" name="SUPPLIER" dataDxfId="5" totalsRowDxfId="4"/>
-    <tableColumn id="14" xr3:uid="{36592479-8EA8-4D42-8DFF-452C7024B605}" name="Price per unit (CHF)" dataDxfId="3" totalsRowDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{E4EF20A8-BAA7-4285-8E2C-1FF15F4D9DE0}" name="QTY" dataDxfId="14" totalsRowDxfId="13"/>
+    <tableColumn id="3" xr3:uid="{7C114C88-4C53-4A01-875E-42C9A5D3836B}" name="PART NR. " dataDxfId="12" totalsRowDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{F56A10FA-89C2-4781-AECC-93B30002C92E}" name="DESCRIPTION" dataDxfId="10" totalsRowDxfId="9"/>
+    <tableColumn id="6" xr3:uid="{15467916-B419-479D-A3A9-C6B2B5C762DF}" name="PRODUCT CODE" dataDxfId="8" totalsRowDxfId="7"/>
+    <tableColumn id="7" xr3:uid="{2349CBB5-C81B-4DFD-9B9F-CC6E1EB0C9BF}" name="SUPPLIER" dataDxfId="6" totalsRowDxfId="5"/>
+    <tableColumn id="14" xr3:uid="{36592479-8EA8-4D42-8DFF-452C7024B605}" name="PRICE PER UNIT (CHF)" dataDxfId="4" totalsRowDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4740,9 +4740,9 @@
     <tableColumn id="3" xr3:uid="{A8C4F21C-CD18-4C55-8F37-A63DC3DADA2A}" name="Length [m]"/>
     <tableColumn id="4" xr3:uid="{58450646-C7B3-41F9-9EA9-C5AC13C9F0E1}" name="QTY to ZHR"/>
     <tableColumn id="5" xr3:uid="{7591EFD4-7391-4754-8536-9BFADAB2E4F8}" name="QTY to BOS"/>
-    <tableColumn id="6" xr3:uid="{62F124C5-9852-4F6A-9A5B-7833BB832B2B}" name="TOTAL QTY" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{62F124C5-9852-4F6A-9A5B-7833BB832B2B}" name="TOTAL QTY" dataDxfId="2"/>
     <tableColumn id="7" xr3:uid="{96FA4321-6955-4909-B76A-703878A5516D}" name="Cost/part [CHF]"/>
-    <tableColumn id="8" xr3:uid="{F9E937AD-E464-40D7-87A7-E2D2618ABCD4}" name="Total [CHF]" totalsRowFunction="sum" dataDxfId="0"/>
+    <tableColumn id="8" xr3:uid="{F9E937AD-E464-40D7-87A7-E2D2618ABCD4}" name="Total [CHF]" totalsRowFunction="sum" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5048,7 +5048,7 @@
   <dimension ref="A1:F55"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -5058,7 +5058,7 @@
     <col min="3" max="3" width="37.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="40.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="35" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="27.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="30" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
@@ -5067,19 +5067,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>4</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>22</v>
+        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -5087,19 +5087,19 @@
         <v>12</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>55</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>25</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -5107,19 +5107,19 @@
         <v>60</v>
       </c>
       <c r="B3" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="D3" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>28</v>
-      </c>
       <c r="F3" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -5127,19 +5127,19 @@
         <v>6</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
@@ -5147,19 +5147,19 @@
         <v>4</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F5" s="5" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="6" spans="1:6" ht="31.5" x14ac:dyDescent="0.25">
@@ -5167,16 +5167,16 @@
         <v>12</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>33</v>
+        <v>56</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F6" s="6">
         <v>3</v>
@@ -5187,19 +5187,19 @@
         <v>4</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -5207,19 +5207,19 @@
         <v>4</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -5227,19 +5227,19 @@
         <v>2</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -5247,19 +5247,19 @@
         <v>4</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="5" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -5267,19 +5267,19 @@
         <v>4</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" spans="1:6" ht="78.75" x14ac:dyDescent="0.25">
@@ -5287,19 +5287,19 @@
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="E12" s="5" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -5307,19 +5307,19 @@
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -5327,19 +5327,19 @@
         <v>2</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -5347,19 +5347,19 @@
         <v>4</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F15" s="6" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -7701,28 +7701,28 @@
   <sheetData>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>14</v>
       </c>
-      <c r="F2" t="s">
-        <v>15</v>
-      </c>
       <c r="G2" t="s">
+        <v>19</v>
+      </c>
+      <c r="H2" t="s">
         <v>20</v>
-      </c>
-      <c r="H2" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
@@ -7733,7 +7733,7 @@
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="H9">
         <f>SUBTOTAL(109,Table2[Total '[CHF']])</f>
@@ -7761,42 +7761,42 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -7951,7 +7951,7 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6732F7FA-6296-4A7E-ACC0-B3550B3D96F7}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{42CC9AC7-53DD-4EA1-94F4-5CED16B8A117}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
     <ds:schemaRef ds:uri="HelblingDocs"/>

</xml_diff>